<commit_message>
Inicio da macro SOD
</commit_message>
<xml_diff>
--- a/assets/excel/plan_teste.xlsx
+++ b/assets/excel/plan_teste.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
-  <si>
-    <t xml:space="preserve">T11 </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+  <si>
+    <t xml:space="preserve">T11</t>
   </si>
   <si>
     <t xml:space="preserve">Prazo T11 </t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Cliente </t>
   </si>
   <si>
-    <t xml:space="preserve">RG </t>
+    <t xml:space="preserve">RG</t>
   </si>
   <si>
     <t xml:space="preserve">TM CIS </t>
@@ -149,6 +149,21 @@
   </si>
   <si>
     <t xml:space="preserve">600/5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRRLOIENTR101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIT SERVICOS DE RADIOLOGIA LTDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASCAVEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200/5</t>
   </si>
 </sst>
 </file>
@@ -401,10 +416,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF4"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -724,8 +739,99 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G4" s="3"/>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>20246940865024</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>45511</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>45511</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>20247061008983</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>45519</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>105086940</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>44630811</v>
+      </c>
+      <c r="K4" s="3" t="n">
+        <v>44702450</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>15508</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>45658</v>
+      </c>
+      <c r="N4" s="4" t="n">
+        <v>45495</v>
+      </c>
+      <c r="O4" s="4" t="n">
+        <v>45495</v>
+      </c>
+      <c r="P4" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="Q4" s="6" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R4" s="6" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" s="3" t="n">
+        <v>61</v>
+      </c>
+      <c r="V4" s="3" t="n">
+        <v>395107003</v>
+      </c>
+      <c r="W4" s="3" t="n">
+        <v>395107005</v>
+      </c>
+      <c r="X4" s="3" t="n">
+        <v>395107046</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Nova interface app dmed
</commit_message>
<xml_diff>
--- a/assets/excel/plan_teste.xlsx
+++ b/assets/excel/plan_teste.xlsx
@@ -418,8 +418,8 @@
   </sheetPr>
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X5" activeCellId="0" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -429,9 +429,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="33.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="39.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="27.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="9.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.72"/>

</xml_diff>

<commit_message>
Versão quase pronta cadastro ccee
</commit_message>
<xml_diff>
--- a/assets/excel/plan_teste.xlsx
+++ b/assets/excel/plan_teste.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="60">
   <si>
     <t xml:space="preserve">T11</t>
   </si>
@@ -188,15 +188,28 @@
   </si>
   <si>
     <t xml:space="preserve">75.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRRRPRENTR101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONFECCOES RAFFER LTDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRANCISCO BELTRAO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">800/5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -287,8 +300,12 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -296,15 +313,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -436,402 +465,402 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AS5"/>
+  <dimension ref="A1:AS6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB12" activeCellId="0" sqref="AB12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="9.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="14.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="17.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="22" style="0" width="10.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="5.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="6.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="42.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="30" style="0" width="16.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="27.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="9.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="14.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="14.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="10.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="9.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="17.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="22" style="1" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="5.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="6.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="42.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="30" style="1" width="16.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>20246906487326</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>45506</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>45506</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>20247035997348</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>45517</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="0" t="s">
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>111001790</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>40622253</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>43701402</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="1" t="n">
         <v>14553</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>45658</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
         <v>45491</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="1" t="n">
         <v>45112</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P2" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="Q2" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="R2" s="1" t="n">
         <v>0.3</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="S2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U2" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="V2" s="0" t="n">
+      <c r="V2" s="1" t="n">
         <v>285515018</v>
       </c>
-      <c r="W2" s="0" t="n">
+      <c r="W2" s="1" t="n">
         <v>285515051</v>
       </c>
-      <c r="X2" s="0" t="n">
+      <c r="X2" s="1" t="n">
         <v>285616256</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="Y2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD2" s="0" t="n">
+      <c r="Z2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD2" s="1" t="n">
         <v>58.3997690242011</v>
       </c>
-      <c r="AE2" s="0" t="n">
+      <c r="AE2" s="1" t="n">
         <v>35.8758532687728</v>
       </c>
-      <c r="AF2" s="0" t="n">
+      <c r="AF2" s="1" t="n">
         <v>99.6311588458663</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>20247618718783</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>45602</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>31620515</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="1" t="n">
         <v>44632005</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>44702609</v>
       </c>
-      <c r="L3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="0" t="n">
+      <c r="L3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="1" t="n">
         <v>45566</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>45587</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="1" t="n">
         <v>45587</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="P3" s="1" t="n">
         <v>225</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="Q3" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="R3" s="0" t="n">
+      <c r="R3" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="S3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="T3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="U3" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="V3" s="1" t="n">
         <v>786021115</v>
       </c>
-      <c r="W3" s="0" t="n">
+      <c r="W3" s="1" t="n">
         <v>816121051</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="Y3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Z3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE3" s="0" t="s">
+      <c r="Z3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>20246940865024</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>45511</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>45511</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>20247061008983</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>45519</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="0" t="s">
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>105086940</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="n">
         <v>44630811</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>44702450</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4" s="1" t="n">
         <v>15508</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="1" t="n">
         <v>45658</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="1" t="n">
         <v>45495</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="O4" s="1" t="n">
         <v>45495</v>
       </c>
-      <c r="P4" s="0" t="n">
+      <c r="P4" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="Q4" s="0" t="n">
+      <c r="Q4" s="1" t="n">
         <v>0.01</v>
       </c>
-      <c r="R4" s="0" t="n">
+      <c r="R4" s="1" t="n">
         <v>0.15</v>
       </c>
-      <c r="S4" s="0" t="s">
+      <c r="S4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T4" s="0" t="s">
+      <c r="T4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U4" s="0" t="n">
+      <c r="U4" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="V4" s="0" t="n">
+      <c r="V4" s="1" t="n">
         <v>395107003</v>
       </c>
-      <c r="W4" s="0" t="n">
+      <c r="W4" s="1" t="n">
         <v>395107005</v>
       </c>
-      <c r="X4" s="0" t="n">
+      <c r="X4" s="1" t="n">
         <v>395107046</v>
       </c>
-      <c r="Y4" s="0" t="s">
+      <c r="Y4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
+      <c r="Z4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
@@ -912,13 +941,13 @@
       <c r="Z5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AA5" s="0" t="s">
+      <c r="AA5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AB5" s="0" t="s">
+      <c r="AB5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AC5" s="0" t="s">
+      <c r="AC5" s="1" t="s">
         <v>55</v>
       </c>
       <c r="AD5" s="2" t="s">
@@ -967,6 +996,110 @@
         <v>32</v>
       </c>
       <c r="AS5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="n">
+        <v>20247553349300</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>45595</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <v>53105028</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="6" t="n">
+        <v>40625264</v>
+      </c>
+      <c r="K6" s="6" t="n">
+        <v>44701768</v>
+      </c>
+      <c r="L6" s="6" t="n">
+        <v>14983</v>
+      </c>
+      <c r="M6" s="8" t="n">
+        <v>45778</v>
+      </c>
+      <c r="N6" s="7" t="n">
+        <v>45579</v>
+      </c>
+      <c r="O6" s="7" t="n">
+        <v>45579</v>
+      </c>
+      <c r="P6" s="9" t="n">
+        <v>300</v>
+      </c>
+      <c r="Q6" s="9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="R6" s="9" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="U6" s="6" t="n">
+        <v>77</v>
+      </c>
+      <c r="V6" s="6" t="n">
+        <v>205824039</v>
+      </c>
+      <c r="W6" s="6" t="n">
+        <v>906224018</v>
+      </c>
+      <c r="X6" s="6" t="n">
+        <v>996124007</v>
+      </c>
+      <c r="Y6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH6" s="6" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>